<commit_message>
Separated languages to make it easier to add more languages later
</commit_message>
<xml_diff>
--- a/Assets/Excel/chapter01.xlsx
+++ b/Assets/Excel/chapter01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ulko\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F765DDCC-3A1A-4D32-AF9B-45939268CE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DE1B6A-6890-4C15-A5D2-A8CD4F4C47A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="2040" windowWidth="22860" windowHeight="15150" tabRatio="856" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2745" yWindow="5190" windowWidth="24255" windowHeight="14475" tabRatio="856" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="50" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
   <si>
     <t>speaker</t>
   </si>
@@ -249,6 +249,21 @@
   </si>
   <si>
     <t>I already regret letting you out.</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>Lorsque les moines ont commencé à mourir d'une maladie mystérieuse, le Dr Ulko est arrivé sur les lieux.</t>
+  </si>
+  <si>
+    <t>Malheureusement pour lui, les moines ont pris l'histoire à l'envers et ont cru que la présence de l'étranger avait causé la maladie, et non que la maladie avait causé la présence de l'étranger. Personne ne sait s'ils avaient raison ou non.</t>
+  </si>
+  <si>
+    <t>Ils décident de l'exiler dans l'Autre Monde...</t>
+  </si>
+  <si>
+    <t>en,fr</t>
   </si>
 </sst>
 </file>
@@ -612,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA164FE-E939-4B46-8D22-A2D4973D15A1}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,6 +648,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -641,7 +661,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA602FF-9F6D-431C-8906-D7B3D2E309D3}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -651,29 +671,42 @@
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="63" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -683,10 +716,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE95CCD-0122-4522-9228-A3B17B3B2FE4}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,25 +728,28 @@
     <col min="2" max="2" width="63" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
@@ -725,10 +761,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6B78FA-F9B7-40E6-ABD2-5B3680262E8B}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,20 +773,23 @@
     <col min="2" max="2" width="63" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -758,12 +797,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -771,7 +810,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -779,7 +818,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -787,7 +826,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -795,7 +834,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -803,7 +842,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -811,12 +850,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -824,12 +863,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -837,12 +876,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -960,10 +999,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF5E5A2-83AF-4099-9057-002EBB6C6BAC}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,20 +1011,23 @@
     <col min="2" max="2" width="63" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -993,7 +1035,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
     </row>
   </sheetData>
@@ -1003,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31AC472B-F34E-499C-ABBA-8590D6D4205E}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,20 +1057,23 @@
     <col min="2" max="2" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1036,7 +1081,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1044,7 +1089,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1052,7 +1097,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1060,7 +1105,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1068,7 +1113,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1076,7 +1121,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1084,7 +1129,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1092,12 +1137,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1105,12 +1150,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1118,12 +1163,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1159,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A94DFF-C8B4-480B-9DB8-3105338ED399}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,20 +1216,23 @@
     <col min="2" max="2" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -1192,7 +1240,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1200,7 +1248,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1208,7 +1256,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1216,7 +1264,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1224,7 +1272,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1232,28 +1280,28 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>